<commit_message>
Schemas and the template endpoint can handle multiple submission types
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.0.xlsx
+++ b/schema_definitions/template_schema_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E9780C-DA5F-3840-9C56-6924698E370A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1B677A-D1EC-7B4F-9508-138D0B036608}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>MANDATORY</t>
-  </si>
-  <si>
     <t>TYPE</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>The GWAS Catalog study accession identifying a published study</t>
+  </si>
+  <si>
+    <t>MANDATORY-METADATA</t>
   </si>
 </sst>
 </file>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,39 +972,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="b">
         <v>1</v>
@@ -1013,19 +1013,19 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
@@ -1033,122 +1033,122 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" t="s">
         <v>155</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>156</v>
-      </c>
-      <c r="J3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="G7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
         <v>46</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -1157,18 +1157,18 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -1177,18 +1177,18 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -1197,18 +1197,18 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1217,21 +1217,21 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -1240,21 +1240,21 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1263,21 +1263,21 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1286,21 +1286,21 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>1</v>
@@ -1309,53 +1309,53 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" t="s">
         <v>68</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
         <v>56</v>
-      </c>
-      <c r="J17" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1371,7 +1371,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,42 +1394,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
@@ -1438,14 +1438,14 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="b">
@@ -1454,10 +1454,10 @@
     </row>
     <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
@@ -1466,14 +1466,14 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="b">
@@ -1482,10 +1482,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>1</v>
@@ -1494,14 +1494,14 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="b">
@@ -1510,10 +1510,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>1</v>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1533,7 +1533,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="b">
@@ -1542,10 +1542,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>1</v>
@@ -1554,14 +1554,14 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="b">
@@ -1570,10 +1570,10 @@
     </row>
     <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
@@ -1582,14 +1582,14 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="b">
@@ -1598,10 +1598,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -1610,26 +1610,26 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -1638,26 +1638,26 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
@@ -1666,24 +1666,24 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
@@ -1692,24 +1692,24 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -1718,24 +1718,24 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>0</v>
@@ -1744,24 +1744,24 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>0</v>
@@ -1770,24 +1770,24 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>0</v>
@@ -1796,24 +1796,24 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>0</v>
@@ -1822,14 +1822,14 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1852,7 +1852,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1878,42 +1878,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>9</v>
-      </c>
       <c r="L1" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="9" t="b">
         <v>1</v>
@@ -1922,21 +1922,21 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="9" t="b">
         <v>1</v>
@@ -1945,22 +1945,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="9"/>
       <c r="J3" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="9" t="b">
         <v>1</v>
@@ -1969,18 +1969,18 @@
         <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="9" t="b">
         <v>1</v>
@@ -1989,18 +1989,18 @@
         <v>0</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="9" t="b">
         <v>1</v>
@@ -2009,18 +2009,18 @@
         <v>0</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="9" t="b">
         <v>1</v>
@@ -2029,21 +2029,21 @@
         <v>0</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="9" t="b">
         <v>1</v>
@@ -2052,21 +2052,21 @@
         <v>1</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="9" t="b">
         <v>1</v>
@@ -2075,18 +2075,18 @@
         <v>0</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="9" t="b">
         <v>1</v>
@@ -2095,18 +2095,18 @@
         <v>0</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="9" t="b">
         <v>1</v>
@@ -2115,13 +2115,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3123,8 +3123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3146,39 +3146,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>0</v>
@@ -3187,15 +3187,15 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="b">
@@ -3205,16 +3205,16 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4"/>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -3223,19 +3223,19 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4"/>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -3244,14 +3244,14 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="4"/>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>